<commit_message>
-- phuc -- fix SRS_CNPM.docx
</commit_message>
<xml_diff>
--- a/CNPM/Appendix2.xlsx
+++ b/CNPM/Appendix2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="26">
   <si>
     <t>FR2</t>
   </si>
@@ -263,45 +263,14 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -324,7 +293,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -426,7 +397,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="dk1">
+                <a:tint val="55000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -479,34 +452,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7.9976926479918085</c:v>
+                  <c:v>19.394238601900707</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.260996845221131</c:v>
+                  <c:v>10.99734757499167</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.459541612822141</c:v>
+                  <c:v>13.277599879507582</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.840783782751567</c:v>
+                  <c:v>10.697129574122288</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.798965203806015</c:v>
+                  <c:v>12.747763917679944</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.8511597155219572</c:v>
+                  <c:v>4.8904585630178579</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.1109271352754364</c:v>
+                  <c:v>3.4497212205069063</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8545063041590955</c:v>
+                  <c:v>2.4153129502686181</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.2949195224760297</c:v>
+                  <c:v>2.7434159627137866</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.530507229974827</c:v>
+                  <c:v>19.387011755290622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,11 +495,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1345423872"/>
-        <c:axId val="-1345435296"/>
+        <c:axId val="2098785120"/>
+        <c:axId val="2098780224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1345423872"/>
+        <c:axId val="2098785120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1345435296"/>
+        <c:crossAx val="2098780224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -577,7 +550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1345435296"/>
+        <c:axId val="2098780224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,49 +601,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1345423872"/>
+        <c:crossAx val="2098785120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -886,7 +820,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7.9976926479918085</c:v>
+                  <c:v>19.394238601900707</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,7 +976,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10.260996845221131</c:v>
+                  <c:v>10.99734757499167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1153,7 +1087,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>14.459541612822141</c:v>
+                  <c:v>13.277599879507582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1309,7 +1243,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>12.840783782751567</c:v>
+                  <c:v>10.697129574122288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1434,7 +1368,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>11.798965203806015</c:v>
+                  <c:v>12.747763917679944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1559,7 +1493,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.1109271352754364</c:v>
+                  <c:v>3.4497212205069063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1684,7 +1618,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.1109271352754364</c:v>
+                  <c:v>3.4497212205069063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1809,7 +1743,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.8545063041590955</c:v>
+                  <c:v>2.4153129502686181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1934,7 +1868,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.2949195224760297</c:v>
+                  <c:v>2.7434159627137866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2059,7 +1993,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>19.530507229974827</c:v>
+                  <c:v>19.387011755290622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2075,11 +2009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1345434752"/>
-        <c:axId val="-1345430944"/>
+        <c:axId val="2098790560"/>
+        <c:axId val="2098784032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1345434752"/>
+        <c:axId val="2098790560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,12 +2126,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1345430944"/>
+        <c:crossAx val="2098784032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1345430944"/>
+        <c:axId val="2098784032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2317,7 +2251,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1345434752"/>
+        <c:crossAx val="2098790560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2367,41 +2301,28 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
   <cs:variation>
-    <a:lumMod val="60000"/>
+    <a:tint val="88500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
+    <a:tint val="55000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
+    <a:tint val="75000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
+    <a:tint val="98500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50000"/>
+    <a:tint val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
+    <a:tint val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
+    <a:tint val="80000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -3783,7 +3704,7 @@
   <dimension ref="B4:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:L14"/>
+      <selection activeCell="C5" sqref="C5:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4963,7 +4884,7 @@
   <dimension ref="B3:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="B3:M14"/>
+      <selection activeCell="B3" sqref="B3:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4974,9 +4895,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
@@ -5027,44 +4946,35 @@
         <v>1</v>
       </c>
       <c r="D4" s="16">
-        <f>1/C5</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E4" s="16">
-        <f>1/C6</f>
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="F4" s="16">
-        <f>1/C7</f>
+        <v>4</v>
+      </c>
+      <c r="G4" s="16">
+        <v>3</v>
+      </c>
+      <c r="H4" s="16">
+        <v>7</v>
+      </c>
+      <c r="I4" s="16">
+        <v>7</v>
+      </c>
+      <c r="J4" s="16">
+        <v>8</v>
+      </c>
+      <c r="K4" s="16">
+        <v>6</v>
+      </c>
+      <c r="L4" s="16">
         <v>0.33333333333333331</v>
-      </c>
-      <c r="G4" s="16">
-        <f>1/C8</f>
-        <v>0.25</v>
-      </c>
-      <c r="H4" s="16">
-        <f>1/C9</f>
-        <v>2</v>
-      </c>
-      <c r="I4" s="16">
-        <f>1/C10</f>
-        <v>2</v>
-      </c>
-      <c r="J4" s="16">
-        <f>1/C11</f>
-        <v>2</v>
-      </c>
-      <c r="K4" s="16">
-        <f>1/C12</f>
-        <v>3</v>
-      </c>
-      <c r="L4" s="16">
-        <f>1/C13</f>
-        <v>0.5</v>
       </c>
       <c r="M4" s="16">
         <f t="shared" ref="M4:M14" si="0">SUM(C4:L4)</f>
-        <v>11.833333333333334</v>
+        <v>39.333333333333336</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>0</v>
@@ -5079,46 +4989,39 @@
         <v>1</v>
       </c>
       <c r="C5" s="16">
-        <v>2</v>
+        <f>1/D4</f>
+        <v>1</v>
       </c>
       <c r="D5" s="16">
         <v>1</v>
       </c>
       <c r="E5" s="16">
-        <f>1/$D6</f>
         <v>0.5</v>
       </c>
       <c r="F5" s="16">
-        <f>1/$D7</f>
         <v>1</v>
       </c>
       <c r="G5" s="16">
-        <f>1/$D8</f>
         <v>0.5</v>
       </c>
       <c r="H5" s="16">
-        <f>1/$D9</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="16">
-        <f>1/$D10</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J5" s="16">
-        <f>1/$D11</f>
+        <v>7</v>
+      </c>
+      <c r="K5" s="16">
         <v>4</v>
       </c>
-      <c r="K5" s="16">
-        <f>1/$D12</f>
-        <v>2</v>
-      </c>
       <c r="L5" s="16">
-        <f>1/$D13</f>
         <v>0.5</v>
       </c>
       <c r="M5" s="16">
         <f t="shared" si="0"/>
-        <v>15.5</v>
+        <v>24.5</v>
       </c>
       <c r="O5" s="17" t="s">
         <v>1</v>
@@ -5133,45 +5036,40 @@
         <v>2</v>
       </c>
       <c r="C6" s="16">
-        <v>4</v>
+        <f>1/E4</f>
+        <v>0.5</v>
       </c>
       <c r="D6" s="16">
+        <f>1/E$6</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
         <v>2</v>
       </c>
-      <c r="E6" s="16">
-        <v>1</v>
-      </c>
-      <c r="F6" s="16">
-        <f>1/$E7</f>
+      <c r="G6" s="16">
         <v>2</v>
       </c>
-      <c r="G6" s="16">
-        <f>1/$E8</f>
-        <v>2</v>
-      </c>
       <c r="H6" s="16">
-        <f>1/$E9</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I6" s="16">
-        <f>1/$E10</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J6" s="16">
-        <f>1/$E11</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K6" s="16">
-        <f>1/$E12</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L6" s="16">
-        <f>1/$E13</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="M6" s="16">
         <f t="shared" si="0"/>
-        <v>20.333333333333332</v>
+        <v>28.833333333333332</v>
       </c>
       <c r="O6" s="17" t="s">
         <v>2</v>
@@ -5186,44 +5084,41 @@
         <v>3</v>
       </c>
       <c r="C7" s="16">
-        <v>3</v>
+        <f>1/F4</f>
+        <v>0.25</v>
       </c>
       <c r="D7" s="16">
-        <v>1</v>
+        <f>1/F$6</f>
+        <v>0.5</v>
       </c>
       <c r="E7" s="16">
-        <v>0.5</v>
+        <f>1/F$7</f>
+        <v>1</v>
       </c>
       <c r="F7" s="16">
         <v>1</v>
       </c>
       <c r="G7" s="16">
-        <f>1/$F8</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H7" s="16">
-        <f>1/F9</f>
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="I7" s="16">
-        <f>1/F10</f>
         <v>5</v>
       </c>
       <c r="J7" s="16">
-        <f>1/F11</f>
+        <v>8</v>
+      </c>
+      <c r="K7" s="16">
         <v>5</v>
       </c>
-      <c r="K7" s="16">
-        <f>1/F12</f>
-        <v>3</v>
-      </c>
       <c r="L7" s="16">
-        <f>1/F13</f>
         <v>0.5</v>
       </c>
       <c r="M7" s="16">
         <f t="shared" si="0"/>
-        <v>20.5</v>
+        <v>27.583333333333336</v>
       </c>
       <c r="O7" s="17" t="s">
         <v>3</v>
@@ -5238,43 +5133,42 @@
         <v>4</v>
       </c>
       <c r="C8" s="16">
-        <v>4</v>
+        <f>1/G4</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D8" s="16">
-        <v>2</v>
+        <f>1/G$6</f>
+        <v>0.5</v>
       </c>
       <c r="E8" s="16">
-        <v>0.5</v>
+        <f>1/G$7</f>
+        <v>3</v>
       </c>
       <c r="F8" s="16">
+        <f>1/G$8</f>
         <v>1</v>
       </c>
       <c r="G8" s="16">
         <v>1</v>
       </c>
       <c r="H8" s="16">
-        <f>1/G9</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I8" s="16">
-        <f>1/G10</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J8" s="16">
-        <f>1/G11</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K8" s="16">
-        <f>1/G12</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L8" s="16">
-        <f>1/G13</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="M8" s="16">
         <f t="shared" si="0"/>
-        <v>18.833333333333332</v>
+        <v>29.166666666666664</v>
       </c>
       <c r="O8" s="17" t="s">
         <v>4</v>
@@ -5289,42 +5183,43 @@
         <v>5</v>
       </c>
       <c r="C9" s="16">
+        <f>1/H4</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="D9" s="16">
+        <f>1/H$6</f>
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="16">
+        <f>1/H$7</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F9" s="16">
+        <f>1/H7</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G9" s="16">
+        <f>1/H8</f>
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="16">
+        <v>1</v>
+      </c>
+      <c r="I9" s="16">
+        <v>3</v>
+      </c>
+      <c r="J9" s="16">
+        <v>4</v>
+      </c>
+      <c r="K9" s="16">
+        <v>3</v>
+      </c>
+      <c r="L9" s="16">
         <v>0.5</v>
-      </c>
-      <c r="D9" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="16">
-        <v>2</v>
-      </c>
-      <c r="G9" s="16">
-        <v>1</v>
-      </c>
-      <c r="H9" s="16">
-        <v>1</v>
-      </c>
-      <c r="I9" s="16">
-        <f>1/H10</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="16">
-        <f>1/H11</f>
-        <v>3</v>
-      </c>
-      <c r="K9" s="16">
-        <f>1/H12</f>
-        <v>1</v>
-      </c>
-      <c r="L9" s="16">
-        <f>1/H13</f>
-        <v>0.33333333333333331</v>
       </c>
       <c r="M9" s="16">
         <f t="shared" si="0"/>
-        <v>10.833333333333334</v>
+        <v>12.376190476190477</v>
       </c>
       <c r="O9" s="17" t="s">
         <v>5</v>
@@ -5339,41 +5234,44 @@
         <v>6</v>
       </c>
       <c r="C10" s="16">
-        <v>0.5</v>
+        <f>1/I4</f>
+        <v>0.14285714285714285</v>
       </c>
       <c r="D10" s="16">
-        <v>0.5</v>
+        <f>1/I$6</f>
+        <v>0.2</v>
       </c>
       <c r="E10" s="16">
-        <v>0.5</v>
+        <f>1/I$7</f>
+        <v>0.2</v>
       </c>
       <c r="F10" s="16">
+        <f>1/I7</f>
         <v>0.2</v>
       </c>
       <c r="G10" s="16">
-        <v>1</v>
+        <f>1/I8</f>
+        <v>0.2</v>
       </c>
       <c r="H10" s="16">
-        <v>1</v>
+        <f>1/I9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I10" s="16">
         <v>1</v>
       </c>
       <c r="J10" s="16">
-        <f>1/I11</f>
         <v>2</v>
       </c>
       <c r="K10" s="16">
-        <f>1/I12</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" s="16">
-        <f>1/I13</f>
         <v>0.5</v>
       </c>
       <c r="M10" s="16">
         <f t="shared" si="0"/>
-        <v>8.1999999999999993</v>
+        <v>6.7761904761904761</v>
       </c>
       <c r="O10" s="17" t="s">
         <v>6</v>
@@ -5388,40 +5286,45 @@
         <v>7</v>
       </c>
       <c r="C11" s="16">
+        <f>1/J4</f>
+        <v>0.125</v>
+      </c>
+      <c r="D11" s="16">
+        <f>1/J$6</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="E11" s="16">
+        <f>1/J$7</f>
+        <v>0.125</v>
+      </c>
+      <c r="F11" s="16">
+        <f>1/J7</f>
+        <v>0.125</v>
+      </c>
+      <c r="G11" s="16">
+        <f>1/J8</f>
+        <v>0.125</v>
+      </c>
+      <c r="H11" s="16">
+        <f>1/J9</f>
+        <v>0.25</v>
+      </c>
+      <c r="I11" s="16">
+        <f>1/J10</f>
         <v>0.5</v>
       </c>
-      <c r="D11" s="16">
-        <v>0.25</v>
-      </c>
-      <c r="E11" s="16">
-        <v>0.25</v>
-      </c>
-      <c r="F11" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="G11" s="16">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H11" s="16">
+      <c r="J11" s="16">
+        <v>1</v>
+      </c>
+      <c r="K11" s="16">
+        <v>2</v>
+      </c>
+      <c r="L11" s="16">
         <v>0.33333333333333331</v>
-      </c>
-      <c r="I11" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="J11" s="16">
-        <v>1</v>
-      </c>
-      <c r="K11" s="16">
-        <f>1/J12</f>
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="16">
-        <f>1/J13</f>
-        <v>0.25</v>
       </c>
       <c r="M11" s="16">
         <f t="shared" si="0"/>
-        <v>3.95</v>
+        <v>4.7261904761904754</v>
       </c>
       <c r="O11" s="17" t="s">
         <v>7</v>
@@ -5436,39 +5339,46 @@
         <v>16</v>
       </c>
       <c r="C12" s="16">
+        <f>1/K4</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D12" s="16">
+        <f>1/K$6</f>
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="16">
+        <f>1/K$7</f>
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="16">
+        <f>1/K7</f>
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="16">
+        <f>1/K8</f>
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="16">
+        <f>1/K9</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D12" s="16">
+      <c r="I12" s="16">
+        <f>1/K10</f>
         <v>0.5</v>
       </c>
-      <c r="E12" s="16">
-        <v>1</v>
-      </c>
-      <c r="F12" s="16">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G12" s="16">
+      <c r="J12" s="16">
+        <f>1/K11</f>
         <v>0.5</v>
       </c>
-      <c r="H12" s="16">
-        <v>1</v>
-      </c>
-      <c r="I12" s="16">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16">
-        <v>2</v>
-      </c>
       <c r="K12" s="16">
         <v>1</v>
       </c>
       <c r="L12" s="16">
-        <f>1/K13</f>
         <v>0.5</v>
       </c>
       <c r="M12" s="16">
         <f t="shared" si="0"/>
-        <v>8.1666666666666661</v>
+        <v>3.8</v>
       </c>
       <c r="O12" s="17" t="s">
         <v>16</v>
@@ -5483,30 +5393,39 @@
         <v>8</v>
       </c>
       <c r="C13" s="16">
+        <f>1/L4</f>
+        <v>3</v>
+      </c>
+      <c r="D13" s="16">
+        <f>1/L$6</f>
+        <v>3</v>
+      </c>
+      <c r="E13" s="16">
+        <f>1/L$7</f>
         <v>2</v>
       </c>
-      <c r="D13" s="16">
+      <c r="F13" s="16">
+        <f>1/L7</f>
         <v>2</v>
       </c>
-      <c r="E13" s="16">
+      <c r="G13" s="16">
+        <f>1/L8</f>
         <v>3</v>
       </c>
-      <c r="F13" s="16">
+      <c r="H13" s="16">
+        <f>1/L9</f>
         <v>2</v>
       </c>
-      <c r="G13" s="16">
+      <c r="I13" s="16">
+        <f>1/L10</f>
+        <v>2</v>
+      </c>
+      <c r="J13" s="16">
+        <f>1/L11</f>
         <v>3</v>
       </c>
-      <c r="H13" s="16">
-        <v>3</v>
-      </c>
-      <c r="I13" s="16">
-        <v>2</v>
-      </c>
-      <c r="J13" s="16">
-        <v>4</v>
-      </c>
       <c r="K13" s="16">
+        <f>1/L12</f>
         <v>2</v>
       </c>
       <c r="L13" s="16">
@@ -5514,7 +5433,7 @@
       </c>
       <c r="M13" s="16">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O13" s="17" t="s">
         <v>8</v>
@@ -5528,47 +5447,47 @@
       <c r="B14" s="20"/>
       <c r="C14" s="16">
         <f t="shared" ref="C14:L14" si="1">SUM(C4:C13)</f>
-        <v>17.833333333333336</v>
+        <v>6.6607142857142856</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="1"/>
-        <v>10.25</v>
+        <v>7.7428571428571438</v>
       </c>
       <c r="E14" s="16">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10.191666666666666</v>
       </c>
       <c r="F14" s="16">
         <f t="shared" si="1"/>
-        <v>10.066666666666666</v>
+        <v>11.691666666666665</v>
       </c>
       <c r="G14" s="16">
         <f t="shared" si="1"/>
-        <v>10.416666666666668</v>
+        <v>10.558333333333334</v>
       </c>
       <c r="H14" s="16">
         <f t="shared" si="1"/>
-        <v>13.833333333333334</v>
+        <v>30.916666666666664</v>
       </c>
       <c r="I14" s="16">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>34</v>
       </c>
       <c r="J14" s="16">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>48.5</v>
       </c>
       <c r="K14" s="16">
         <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>35</v>
       </c>
       <c r="L14" s="16">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>4.8333333333333339</v>
       </c>
       <c r="M14" s="16">
         <f t="shared" si="0"/>
-        <v>142.15</v>
+        <v>200.0952380952381</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
@@ -5612,47 +5531,47 @@
       </c>
       <c r="C17" s="21">
         <f>C4/C$14</f>
-        <v>5.6074766355140179E-2</v>
+        <v>0.15013404825737264</v>
       </c>
       <c r="D17" s="21">
         <f>D4/D$14</f>
-        <v>4.878048780487805E-2</v>
+        <v>0.1291512915129151</v>
       </c>
       <c r="E17" s="21">
         <f t="shared" ref="E17:L17" si="2">E4/E$14</f>
-        <v>3.125E-2</v>
+        <v>0.19623875715453803</v>
       </c>
       <c r="F17" s="21">
         <f t="shared" si="2"/>
-        <v>3.3112582781456949E-2</v>
+        <v>0.34212401995723457</v>
       </c>
       <c r="G17" s="21">
         <f t="shared" si="2"/>
-        <v>2.3999999999999997E-2</v>
+        <v>0.2841357537490134</v>
       </c>
       <c r="H17" s="21">
         <f t="shared" si="2"/>
-        <v>0.14457831325301204</v>
+        <v>0.22641509433962265</v>
       </c>
       <c r="I17" s="21">
         <f t="shared" si="2"/>
-        <v>0.11428571428571428</v>
+        <v>0.20588235294117646</v>
       </c>
       <c r="J17" s="21">
         <f t="shared" si="2"/>
-        <v>6.0606060606060608E-2</v>
+        <v>0.16494845360824742</v>
       </c>
       <c r="K17" s="21">
         <f t="shared" si="2"/>
-        <v>0.18181818181818182</v>
+        <v>0.17142857142857143</v>
       </c>
       <c r="L17" s="21">
         <f t="shared" si="2"/>
-        <v>0.10526315789473684</v>
+        <v>6.8965517241379296E-2</v>
       </c>
       <c r="M17" s="21">
         <f t="shared" ref="M17:M27" si="3">SUM(C17:L17)</f>
-        <v>0.79976926479918087</v>
+        <v>1.9394238601900711</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -5661,47 +5580,47 @@
       </c>
       <c r="C18" s="21">
         <f t="shared" ref="C18:L27" si="4">C5/C$14</f>
-        <v>0.11214953271028036</v>
+        <v>0.15013404825737264</v>
       </c>
       <c r="D18" s="21">
         <f t="shared" si="4"/>
-        <v>9.7560975609756101E-2</v>
+        <v>0.1291512915129151</v>
       </c>
       <c r="E18" s="21">
         <f t="shared" si="4"/>
-        <v>6.25E-2</v>
+        <v>4.9059689288634509E-2</v>
       </c>
       <c r="F18" s="21">
         <f t="shared" si="4"/>
-        <v>9.9337748344370869E-2</v>
+        <v>8.5531004989308643E-2</v>
       </c>
       <c r="G18" s="21">
         <f t="shared" si="4"/>
-        <v>4.7999999999999994E-2</v>
+        <v>4.7355958958168902E-2</v>
       </c>
       <c r="H18" s="21">
         <f t="shared" si="4"/>
-        <v>0.14457831325301204</v>
+        <v>0.1293800539083558</v>
       </c>
       <c r="I18" s="21">
         <f t="shared" si="4"/>
+        <v>0.14705882352941177</v>
+      </c>
+      <c r="J18" s="21">
+        <f t="shared" si="4"/>
+        <v>0.14432989690721648</v>
+      </c>
+      <c r="K18" s="21">
+        <f t="shared" si="4"/>
         <v>0.11428571428571428</v>
       </c>
-      <c r="J18" s="21">
-        <f t="shared" si="4"/>
-        <v>0.12121212121212122</v>
-      </c>
-      <c r="K18" s="21">
-        <f t="shared" si="4"/>
-        <v>0.12121212121212122</v>
-      </c>
       <c r="L18" s="21">
         <f t="shared" si="4"/>
-        <v>0.10526315789473684</v>
+        <v>0.10344827586206895</v>
       </c>
       <c r="M18" s="21">
         <f t="shared" si="3"/>
-        <v>1.0260996845221131</v>
+        <v>1.0997347574991672</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -5710,47 +5629,47 @@
       </c>
       <c r="C19" s="21">
         <f t="shared" si="4"/>
-        <v>0.22429906542056072</v>
+        <v>7.5067024128686322E-2</v>
       </c>
       <c r="D19" s="21">
         <f t="shared" si="4"/>
-        <v>0.1951219512195122</v>
+        <v>0.1291512915129151</v>
       </c>
       <c r="E19" s="21">
         <f t="shared" si="4"/>
-        <v>0.125</v>
+        <v>9.8119378577269017E-2</v>
       </c>
       <c r="F19" s="21">
         <f t="shared" si="4"/>
-        <v>0.19867549668874174</v>
+        <v>0.17106200997861729</v>
       </c>
       <c r="G19" s="21">
         <f t="shared" si="4"/>
-        <v>0.19199999999999998</v>
+        <v>0.18942383583267561</v>
       </c>
       <c r="H19" s="21">
         <f t="shared" si="4"/>
-        <v>0.14457831325301204</v>
+        <v>0.16172506738544476</v>
       </c>
       <c r="I19" s="21">
         <f t="shared" si="4"/>
-        <v>0.11428571428571428</v>
+        <v>0.14705882352941177</v>
       </c>
       <c r="J19" s="21">
         <f t="shared" si="4"/>
-        <v>0.12121212121212122</v>
+        <v>0.14432989690721648</v>
       </c>
       <c r="K19" s="21">
         <f t="shared" si="4"/>
-        <v>6.0606060606060608E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="L19" s="21">
         <f t="shared" si="4"/>
-        <v>7.0175438596491224E-2</v>
+        <v>6.8965517241379296E-2</v>
       </c>
       <c r="M19" s="21">
         <f t="shared" si="3"/>
-        <v>1.445954161282214</v>
+        <v>1.3277599879507584</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
@@ -5759,47 +5678,47 @@
       </c>
       <c r="C20" s="21">
         <f t="shared" si="4"/>
-        <v>0.16822429906542055</v>
+        <v>3.7533512064343161E-2</v>
       </c>
       <c r="D20" s="21">
         <f t="shared" si="4"/>
-        <v>9.7560975609756101E-2</v>
+        <v>6.457564575645755E-2</v>
       </c>
       <c r="E20" s="21">
         <f t="shared" si="4"/>
-        <v>6.25E-2</v>
+        <v>9.8119378577269017E-2</v>
       </c>
       <c r="F20" s="21">
         <f t="shared" si="4"/>
-        <v>9.9337748344370869E-2</v>
+        <v>8.5531004989308643E-2</v>
       </c>
       <c r="G20" s="21">
         <f t="shared" si="4"/>
-        <v>9.5999999999999988E-2</v>
+        <v>3.157063930544593E-2</v>
       </c>
       <c r="H20" s="21">
         <f t="shared" si="4"/>
-        <v>3.614457831325301E-2</v>
+        <v>0.19407008086253372</v>
       </c>
       <c r="I20" s="21">
         <f t="shared" si="4"/>
-        <v>0.2857142857142857</v>
+        <v>0.14705882352941177</v>
       </c>
       <c r="J20" s="21">
         <f t="shared" si="4"/>
-        <v>0.15151515151515152</v>
+        <v>0.16494845360824742</v>
       </c>
       <c r="K20" s="21">
         <f t="shared" si="4"/>
-        <v>0.18181818181818182</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="L20" s="21">
         <f t="shared" si="4"/>
-        <v>0.10526315789473684</v>
+        <v>0.10344827586206895</v>
       </c>
       <c r="M20" s="21">
         <f t="shared" si="3"/>
-        <v>1.2840783782751566</v>
+        <v>1.069712957412229</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -5808,47 +5727,47 @@
       </c>
       <c r="C21" s="21">
         <f t="shared" si="4"/>
-        <v>0.22429906542056072</v>
+        <v>5.0044682752457548E-2</v>
       </c>
       <c r="D21" s="21">
         <f t="shared" si="4"/>
-        <v>0.1951219512195122</v>
+        <v>6.457564575645755E-2</v>
       </c>
       <c r="E21" s="21">
         <f t="shared" si="4"/>
-        <v>6.25E-2</v>
+        <v>0.29435813573180702</v>
       </c>
       <c r="F21" s="21">
         <f t="shared" si="4"/>
-        <v>9.9337748344370869E-2</v>
+        <v>8.5531004989308643E-2</v>
       </c>
       <c r="G21" s="21">
         <f t="shared" si="4"/>
-        <v>9.5999999999999988E-2</v>
+        <v>9.4711917916337804E-2</v>
       </c>
       <c r="H21" s="21">
         <f t="shared" si="4"/>
-        <v>7.2289156626506021E-2</v>
+        <v>0.16172506738544476</v>
       </c>
       <c r="I21" s="21">
         <f t="shared" si="4"/>
-        <v>5.7142857142857141E-2</v>
+        <v>0.14705882352941177</v>
       </c>
       <c r="J21" s="21">
         <f t="shared" si="4"/>
-        <v>0.18181818181818182</v>
+        <v>0.16494845360824742</v>
       </c>
       <c r="K21" s="21">
         <f t="shared" si="4"/>
-        <v>0.12121212121212122</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="L21" s="21">
         <f t="shared" si="4"/>
-        <v>7.0175438596491224E-2</v>
+        <v>6.8965517241379296E-2</v>
       </c>
       <c r="M21" s="21">
         <f t="shared" si="3"/>
-        <v>1.1798965203806013</v>
+        <v>1.2747763917679946</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -5857,47 +5776,47 @@
       </c>
       <c r="C22" s="21">
         <f t="shared" si="4"/>
-        <v>2.803738317757009E-2</v>
+        <v>2.1447721179624665E-2</v>
       </c>
       <c r="D22" s="21">
         <f t="shared" si="4"/>
-        <v>4.878048780487805E-2</v>
+        <v>2.5830258302583023E-2</v>
       </c>
       <c r="E22" s="21">
         <f t="shared" si="4"/>
-        <v>6.25E-2</v>
+        <v>1.6353229762878167E-2</v>
       </c>
       <c r="F22" s="21">
         <f t="shared" si="4"/>
-        <v>0.19867549668874174</v>
+        <v>1.4255167498218107E-2</v>
       </c>
       <c r="G22" s="21">
         <f t="shared" si="4"/>
-        <v>9.5999999999999988E-2</v>
+        <v>1.8942383583267563E-2</v>
       </c>
       <c r="H22" s="21">
         <f t="shared" si="4"/>
-        <v>7.2289156626506021E-2</v>
+        <v>3.2345013477088951E-2</v>
       </c>
       <c r="I22" s="21">
         <f t="shared" si="4"/>
-        <v>5.7142857142857141E-2</v>
+        <v>8.8235294117647065E-2</v>
       </c>
       <c r="J22" s="21">
         <f t="shared" si="4"/>
-        <v>9.0909090909090912E-2</v>
+        <v>8.247422680412371E-2</v>
       </c>
       <c r="K22" s="21">
         <f t="shared" si="4"/>
-        <v>6.0606060606060608E-2</v>
+        <v>8.5714285714285715E-2</v>
       </c>
       <c r="L22" s="21">
         <f t="shared" si="4"/>
-        <v>7.0175438596491224E-2</v>
+        <v>0.10344827586206895</v>
       </c>
       <c r="M22" s="21">
         <f t="shared" si="3"/>
-        <v>0.78511597155219581</v>
+        <v>0.48904585630178588</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
@@ -5906,47 +5825,47 @@
       </c>
       <c r="C23" s="21">
         <f t="shared" si="4"/>
-        <v>2.803738317757009E-2</v>
+        <v>2.1447721179624665E-2</v>
       </c>
       <c r="D23" s="21">
         <f t="shared" si="4"/>
-        <v>4.878048780487805E-2</v>
+        <v>2.5830258302583023E-2</v>
       </c>
       <c r="E23" s="21">
         <f t="shared" si="4"/>
-        <v>6.25E-2</v>
+        <v>1.9623875715453803E-2</v>
       </c>
       <c r="F23" s="21">
         <f t="shared" si="4"/>
-        <v>1.9867549668874173E-2</v>
+        <v>1.7106200997861729E-2</v>
       </c>
       <c r="G23" s="21">
         <f t="shared" si="4"/>
-        <v>9.5999999999999988E-2</v>
+        <v>1.8942383583267563E-2</v>
       </c>
       <c r="H23" s="21">
         <f t="shared" si="4"/>
-        <v>7.2289156626506021E-2</v>
+        <v>1.078167115902965E-2</v>
       </c>
       <c r="I23" s="21">
         <f t="shared" si="4"/>
+        <v>2.9411764705882353E-2</v>
+      </c>
+      <c r="J23" s="21">
+        <f t="shared" si="4"/>
+        <v>4.1237113402061855E-2</v>
+      </c>
+      <c r="K23" s="21">
+        <f t="shared" si="4"/>
         <v>5.7142857142857141E-2</v>
       </c>
-      <c r="J23" s="21">
-        <f t="shared" si="4"/>
-        <v>6.0606060606060608E-2</v>
-      </c>
-      <c r="K23" s="21">
-        <f t="shared" si="4"/>
-        <v>6.0606060606060608E-2</v>
-      </c>
       <c r="L23" s="21">
         <f t="shared" si="4"/>
-        <v>0.10526315789473684</v>
+        <v>0.10344827586206895</v>
       </c>
       <c r="M23" s="21">
         <f t="shared" si="3"/>
-        <v>0.61109271352754357</v>
+        <v>0.34497212205069072</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
@@ -5955,47 +5874,47 @@
       </c>
       <c r="C24" s="21">
         <f t="shared" si="4"/>
-        <v>2.803738317757009E-2</v>
+        <v>1.876675603217158E-2</v>
       </c>
       <c r="D24" s="21">
         <f t="shared" si="4"/>
-        <v>2.4390243902439025E-2</v>
+        <v>1.8450184501845015E-2</v>
       </c>
       <c r="E24" s="21">
         <f t="shared" si="4"/>
-        <v>3.125E-2</v>
+        <v>1.2264922322158627E-2</v>
       </c>
       <c r="F24" s="21">
         <f t="shared" si="4"/>
-        <v>1.9867549668874173E-2</v>
+        <v>1.069137562366358E-2</v>
       </c>
       <c r="G24" s="21">
         <f t="shared" si="4"/>
-        <v>1.5999999999999997E-2</v>
+        <v>1.1838989739542225E-2</v>
       </c>
       <c r="H24" s="21">
         <f t="shared" si="4"/>
-        <v>2.4096385542168672E-2</v>
+        <v>8.0862533692722376E-3</v>
       </c>
       <c r="I24" s="21">
         <f t="shared" si="4"/>
-        <v>2.8571428571428571E-2</v>
+        <v>1.4705882352941176E-2</v>
       </c>
       <c r="J24" s="21">
         <f t="shared" si="4"/>
-        <v>3.0303030303030304E-2</v>
+        <v>2.0618556701030927E-2</v>
       </c>
       <c r="K24" s="21">
         <f t="shared" si="4"/>
-        <v>3.0303030303030304E-2</v>
+        <v>5.7142857142857141E-2</v>
       </c>
       <c r="L24" s="21">
         <f t="shared" si="4"/>
-        <v>5.2631578947368418E-2</v>
+        <v>6.8965517241379296E-2</v>
       </c>
       <c r="M24" s="21">
         <f t="shared" si="3"/>
-        <v>0.28545063041590957</v>
+        <v>0.24153129502686183</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
@@ -6004,47 +5923,47 @@
       </c>
       <c r="C25" s="21">
         <f t="shared" si="4"/>
-        <v>1.8691588785046724E-2</v>
+        <v>2.5022341376228774E-2</v>
       </c>
       <c r="D25" s="21">
         <f t="shared" si="4"/>
-        <v>4.878048780487805E-2</v>
+        <v>2.5830258302583023E-2</v>
       </c>
       <c r="E25" s="21">
         <f t="shared" si="4"/>
-        <v>0.125</v>
+        <v>1.9623875715453803E-2</v>
       </c>
       <c r="F25" s="21">
         <f t="shared" si="4"/>
-        <v>3.3112582781456949E-2</v>
+        <v>1.7106200997861729E-2</v>
       </c>
       <c r="G25" s="21">
         <f t="shared" si="4"/>
-        <v>4.7999999999999994E-2</v>
+        <v>1.8942383583267563E-2</v>
       </c>
       <c r="H25" s="21">
         <f t="shared" si="4"/>
-        <v>7.2289156626506021E-2</v>
+        <v>1.078167115902965E-2</v>
       </c>
       <c r="I25" s="21">
         <f t="shared" si="4"/>
-        <v>5.7142857142857141E-2</v>
+        <v>1.4705882352941176E-2</v>
       </c>
       <c r="J25" s="21">
         <f t="shared" si="4"/>
-        <v>6.0606060606060608E-2</v>
+        <v>1.0309278350515464E-2</v>
       </c>
       <c r="K25" s="21">
         <f t="shared" si="4"/>
-        <v>6.0606060606060608E-2</v>
+        <v>2.8571428571428571E-2</v>
       </c>
       <c r="L25" s="21">
         <f t="shared" si="4"/>
-        <v>0.10526315789473684</v>
+        <v>0.10344827586206895</v>
       </c>
       <c r="M25" s="21">
         <f t="shared" si="3"/>
-        <v>0.6294919522476029</v>
+        <v>0.27434159627137872</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
@@ -6053,47 +5972,47 @@
       </c>
       <c r="C26" s="21">
         <f t="shared" si="4"/>
-        <v>0.11214953271028036</v>
+        <v>0.45040214477211798</v>
       </c>
       <c r="D26" s="21">
         <f t="shared" si="4"/>
-        <v>0.1951219512195122</v>
+        <v>0.38745387453874536</v>
       </c>
       <c r="E26" s="21">
         <f t="shared" si="4"/>
-        <v>0.375</v>
+        <v>0.19623875715453803</v>
       </c>
       <c r="F26" s="21">
         <f t="shared" si="4"/>
-        <v>0.19867549668874174</v>
+        <v>0.17106200997861729</v>
       </c>
       <c r="G26" s="21">
         <f t="shared" si="4"/>
-        <v>0.28799999999999998</v>
+        <v>0.2841357537490134</v>
       </c>
       <c r="H26" s="21">
         <f t="shared" si="4"/>
-        <v>0.21686746987951808</v>
+        <v>6.4690026954177901E-2</v>
       </c>
       <c r="I26" s="21">
         <f t="shared" si="4"/>
-        <v>0.11428571428571428</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="J26" s="21">
         <f t="shared" si="4"/>
-        <v>0.12121212121212122</v>
+        <v>6.1855670103092786E-2</v>
       </c>
       <c r="K26" s="21">
         <f t="shared" si="4"/>
-        <v>0.12121212121212122</v>
+        <v>5.7142857142857141E-2</v>
       </c>
       <c r="L26" s="21">
         <f t="shared" si="4"/>
-        <v>0.21052631578947367</v>
+        <v>0.2068965517241379</v>
       </c>
       <c r="M26" s="21">
         <f t="shared" si="3"/>
-        <v>1.9530507229974827</v>
+        <v>1.9387011755290626</v>
       </c>
     </row>
     <row r="27" spans="2:13" s="23" customFormat="1" x14ac:dyDescent="0.25">
@@ -6104,7 +6023,7 @@
       </c>
       <c r="D27" s="21">
         <f t="shared" ref="D27:L27" si="5">SUM(D17:D26)</f>
-        <v>1.0000000000000002</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="E27" s="21">
         <f t="shared" si="5"/>
@@ -6112,7 +6031,7 @@
       </c>
       <c r="F27" s="21">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G27" s="21">
         <f t="shared" si="5"/>
@@ -6132,7 +6051,7 @@
       </c>
       <c r="K27" s="21">
         <f t="shared" si="5"/>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="L27" s="21">
         <f t="shared" si="5"/>
@@ -6153,7 +6072,7 @@
   <dimension ref="B1:R28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7342,8 +7261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7425,38 +7344,38 @@
         <v>24</v>
       </c>
       <c r="B5" s="4">
-        <v>0.79976926479918087</v>
+        <v>1.9394238601900711</v>
       </c>
       <c r="C5" s="4">
-        <v>1.0260996845221131</v>
+        <v>1.0997347574991672</v>
       </c>
       <c r="D5" s="4">
-        <v>1.445954161282214</v>
+        <v>1.3277599879507584</v>
       </c>
       <c r="E5" s="4">
-        <v>1.2840783782751566</v>
+        <v>1.069712957412229</v>
       </c>
       <c r="F5" s="4">
-        <v>1.1798965203806013</v>
+        <v>1.2747763917679946</v>
       </c>
       <c r="G5" s="4">
-        <v>0.78511597155219581</v>
+        <v>0.48904585630178588</v>
       </c>
       <c r="H5" s="4">
-        <v>0.61109271352754357</v>
+        <v>0.34497212205069072</v>
       </c>
       <c r="I5" s="4">
-        <v>0.28545063041590957</v>
+        <v>0.24153129502686183</v>
       </c>
       <c r="J5" s="4">
-        <v>0.6294919522476029</v>
+        <v>0.27434159627137872</v>
       </c>
       <c r="K5" s="4">
-        <v>1.9530507229974827</v>
+        <v>1.9387011755290626</v>
       </c>
       <c r="L5" s="11">
         <f>SUM(B5:K5)</f>
-        <v>10</v>
+        <v>10.000000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -7547,47 +7466,47 @@
       </c>
       <c r="B9" s="4">
         <f>(B5/$L$5)*100</f>
-        <v>7.9976926479918085</v>
+        <v>19.394238601900707</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" ref="C9:K9" si="1">(C5/$L$5)*100</f>
-        <v>10.260996845221131</v>
+        <v>10.99734757499167</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="1"/>
-        <v>14.459541612822141</v>
+        <v>13.277599879507582</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>12.840783782751567</v>
+        <v>10.697129574122288</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>11.798965203806015</v>
+        <v>12.747763917679944</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="1"/>
-        <v>7.8511597155219572</v>
+        <v>4.8904585630178579</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="1"/>
-        <v>6.1109271352754364</v>
+        <v>3.4497212205069063</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" si="1"/>
-        <v>2.8545063041590955</v>
+        <v>2.4153129502686181</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="1"/>
-        <v>6.2949195224760297</v>
+        <v>2.7434159627137866</v>
       </c>
       <c r="K9" s="4">
         <f t="shared" si="1"/>
-        <v>19.530507229974827</v>
+        <v>19.387011755290622</v>
       </c>
       <c r="L9" s="11">
         <f>SUM(B9:K9)</f>
-        <v>100.00000000000001</v>
+        <v>99.999999999999972</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-- PHUC -- commit
</commit_message>
<xml_diff>
--- a/CNPM/Appendix2.xlsx
+++ b/CNPM/Appendix2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="27">
   <si>
     <t>FR2</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>TYPE</t>
+  </si>
+  <si>
+    <t>FR9</t>
   </si>
 </sst>
 </file>
@@ -321,7 +324,7 @@
                   <c:v>FR5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>FR11</c:v>
+                  <c:v>FR9</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>QR6</c:v>
@@ -425,7 +428,7 @@
                   <c:v>FR5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>FR11</c:v>
+                  <c:v>FR9</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>QR6</c:v>
@@ -495,11 +498,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2098785120"/>
-        <c:axId val="2098780224"/>
+        <c:axId val="7407408"/>
+        <c:axId val="7405232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2098785120"/>
+        <c:axId val="7407408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2098780224"/>
+        <c:crossAx val="7405232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2098780224"/>
+        <c:axId val="7405232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -601,7 +604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2098785120"/>
+        <c:crossAx val="7407408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1259,7 +1262,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FR11</c:v>
+                  <c:v>FR9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2009,11 +2012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2098790560"/>
-        <c:axId val="2098784032"/>
+        <c:axId val="7397616"/>
+        <c:axId val="7395440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2098790560"/>
+        <c:axId val="7397616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2126,12 +2129,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2098784032"/>
+        <c:crossAx val="7395440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2098784032"/>
+        <c:axId val="7395440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2251,7 +2254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2098790560"/>
+        <c:crossAx val="7397616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4909,7 +4912,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>5</v>
@@ -5505,7 +5508,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H16" s="13" t="s">
         <v>5</v>
@@ -6118,7 +6121,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>5</v>
@@ -6324,7 +6327,7 @@
         <v>14.583333333333334</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>15</v>
@@ -6695,7 +6698,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>5</v>
@@ -7262,7 +7265,7 @@
   <dimension ref="A3:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:K9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7282,7 +7285,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>5</v>
@@ -7393,7 +7396,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
-- phuc -- review
</commit_message>
<xml_diff>
--- a/CNPM/Appendix2.xlsx
+++ b/CNPM/Appendix2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="demo" sheetId="1" r:id="rId1"/>
@@ -498,11 +498,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="7407408"/>
-        <c:axId val="7405232"/>
+        <c:axId val="1939687344"/>
+        <c:axId val="1939679184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="7407408"/>
+        <c:axId val="1939687344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7405232"/>
+        <c:crossAx val="1939679184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -553,7 +553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7405232"/>
+        <c:axId val="1939679184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7407408"/>
+        <c:crossAx val="1939687344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2012,11 +2012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="7397616"/>
-        <c:axId val="7395440"/>
+        <c:axId val="1939673744"/>
+        <c:axId val="1939681904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="7397616"/>
+        <c:axId val="1939673744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2129,12 +2129,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7395440"/>
+        <c:crossAx val="1939681904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="7395440"/>
+        <c:axId val="1939681904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2254,7 +2254,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7397616"/>
+        <c:crossAx val="1939673744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3438,6 +3438,278 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>140805</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>91108</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>74543</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6882848" y="2435087"/>
+          <a:ext cx="1789043" cy="2020956"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>124240</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>173935</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>57978</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6866283" y="3412435"/>
+          <a:ext cx="3611217" cy="1068456"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66261</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>596348</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7421218" y="2675283"/>
+          <a:ext cx="530087" cy="265043"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>HIGH</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19879</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>94422</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>173934</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>168965</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9213575" y="3142422"/>
+          <a:ext cx="766968" cy="265043"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>MEDIUM</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>425727</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342901</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>102704</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9619423" y="3838161"/>
+          <a:ext cx="530087" cy="265043"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>LOW</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7264,8 +7536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>